<commit_message>
update various files for 2016
</commit_message>
<xml_diff>
--- a/support/schedule/eec134-schedule.xlsx
+++ b/support/schedule/eec134-schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Lec/Lab</t>
   </si>
@@ -35,60 +35,9 @@
     <t>Instructor/TA Actions</t>
   </si>
   <si>
-    <t>Lab 1-1-F (Electronics)</t>
-  </si>
-  <si>
-    <t>Lab 1-1-M (Electronics)</t>
-  </si>
-  <si>
-    <t>Lab 1-2-F (Electronics)</t>
-  </si>
-  <si>
-    <t>Lab 1-2-M (Electronics)</t>
-  </si>
-  <si>
-    <t>Lab 1-3-F (Electronics)</t>
-  </si>
-  <si>
-    <t>Lab 1-3-M (Electronics)</t>
-  </si>
-  <si>
-    <t>Lab 3-F (Osc)</t>
-  </si>
-  <si>
-    <t>Lab 3-M (Osc)</t>
-  </si>
-  <si>
-    <t>Lab 4-M (Mixer)</t>
-  </si>
-  <si>
-    <t>Lab 4-F (Mixer)</t>
-  </si>
-  <si>
-    <t>Lab 5-F (Antenna)</t>
-  </si>
-  <si>
-    <t>Lab 6-F (System)</t>
-  </si>
-  <si>
-    <t>Lab 6-M (System)</t>
-  </si>
-  <si>
     <t>Field test</t>
   </si>
   <si>
-    <t>Lab 2-1-F (Amp)</t>
-  </si>
-  <si>
-    <t>Lab 2-1-M (Amp)</t>
-  </si>
-  <si>
-    <t>Lab 2-2-F (Amp)</t>
-  </si>
-  <si>
-    <t>Lab 2-2-M (Amp)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lab Report Due </t>
   </si>
   <si>
@@ -170,27 +119,51 @@
     <t>Submit  by Wednesday (Oct. 28)</t>
   </si>
   <si>
-    <t>Submit overall by Wednesday (Nov. 4)</t>
+    <t>Pre-lab 2.1</t>
+  </si>
+  <si>
+    <t>Pre-lab 2.2</t>
+  </si>
+  <si>
+    <t>Lab 1-1 (Electronics)</t>
+  </si>
+  <si>
+    <t>Lab 1-2 (Electronics)</t>
+  </si>
+  <si>
+    <t>Lab 1-3 (Electronics)</t>
+  </si>
+  <si>
+    <t>Lab 2-1 (Amp)</t>
+  </si>
+  <si>
+    <t>Lab 2-2 (Amp)</t>
+  </si>
+  <si>
+    <t>Lab 3 (Osc)</t>
+  </si>
+  <si>
+    <t>Lab 5 (Antenna)</t>
+  </si>
+  <si>
+    <t>Lab 4 (Mixer)</t>
+  </si>
+  <si>
+    <t>Lab 6 (System)</t>
   </si>
   <si>
     <t>Review files and give initial feedback over the weekend;
-Submit overall by next Wednesday (Nov. 11);
+Submit overall by next Wednesday;
 PCB 1 back</t>
   </si>
   <si>
-    <t>Pre-lab 2.1</t>
-  </si>
-  <si>
-    <t>Pre-lab 2.2</t>
-  </si>
-  <si>
-    <t>Lab 5-M (Antenna)</t>
+    <t>Submit overall by Wednesday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,6 +477,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -539,6 +529,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -698,7 +705,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -727,13 +734,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>38</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>2</v>
@@ -749,13 +756,11 @@
     </row>
     <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>42272</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>3</v>
-      </c>
+        <v>42642</v>
+      </c>
+      <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -763,10 +768,10 @@
     </row>
     <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
-        <v>42275</v>
+        <v>42643</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -783,13 +788,11 @@
     </row>
     <row r="8" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
-        <v>42279</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>5</v>
-      </c>
+        <v>42649</v>
+      </c>
+      <c r="B8" s="17"/>
       <c r="C8" s="17" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -797,10 +800,10 @@
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
-        <v>42282</v>
+        <v>42650</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -817,13 +820,11 @@
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
-        <v>42286</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>7</v>
-      </c>
+        <v>42656</v>
+      </c>
+      <c r="B11" s="11"/>
       <c r="C11" s="11" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
@@ -831,10 +832,10 @@
     </row>
     <row r="12" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
-        <v>42289</v>
+        <v>42657</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -851,26 +852,24 @@
     </row>
     <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
-        <v>42293</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>17</v>
-      </c>
+        <v>42663</v>
+      </c>
+      <c r="B14" s="11"/>
       <c r="C14" s="11" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
-        <v>42296</v>
+        <v>42298</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -887,34 +886,32 @@
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
-        <v>42300</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>19</v>
-      </c>
+        <v>42670</v>
+      </c>
+      <c r="B17" s="11"/>
       <c r="C17" s="11" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
-        <v>42303</v>
+        <v>42305</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="12" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -927,36 +924,34 @@
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
-        <v>42307</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>9</v>
-      </c>
+        <v>42677</v>
+      </c>
+      <c r="B20" s="11"/>
       <c r="C20" s="11" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
-        <v>42310</v>
+        <v>42678</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -969,30 +964,28 @@
     </row>
     <row r="23" spans="1:6" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
-        <v>42314</v>
-      </c>
-      <c r="B23" s="11" t="s">
+        <v>42684</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="F23" s="23" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
-        <v>42317</v>
+        <v>42685</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -1009,30 +1002,28 @@
     </row>
     <row r="26" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
-        <v>42321</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>42691</v>
+      </c>
+      <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D26" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
-        <v>42324</v>
+        <v>42692</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -1049,30 +1040,28 @@
     </row>
     <row r="29" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
-        <v>42328</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>14</v>
-      </c>
+        <v>42698</v>
+      </c>
+      <c r="B29" s="11"/>
       <c r="C29" s="11" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
-        <v>42331</v>
+        <v>42699</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -1089,24 +1078,24 @@
     </row>
     <row r="32" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
-        <v>42335</v>
+        <v>42705</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="11" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="F32" s="12"/>
     </row>
     <row r="33" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
-        <v>42338</v>
+        <v>42706</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -1123,12 +1112,12 @@
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
-        <v>42342</v>
+        <v>42346</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E35" s="19"/>
       <c r="F35" s="12"/>
@@ -1138,7 +1127,7 @@
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="12"/>
@@ -1148,7 +1137,7 @@
     <mergeCell ref="F23:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="74" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="75" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;C&amp;"Book Antiqua,Bold"&amp;18EEC 134A Schedule
 Fall 2015&amp;"-,Regular"

</xml_diff>